<commit_message>
try to fix time series
</commit_message>
<xml_diff>
--- a/example/kerber_landnetz_fl2/scenarios/pv.xlsx
+++ b/example/kerber_landnetz_fl2/scenarios/pv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chujiahe/Desktop/propens-pandapower/example/kerber_landnetz_fl2/scenarios/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B96B1E15-2FB6-A541-AD78-C7EAEB649779}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B81B227-E153-0941-BD08-DB5E2AAD645A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8600" yWindow="640" windowWidth="28040" windowHeight="17420" activeTab="7" xr2:uid="{2084B393-6D21-FD4B-B70D-EA7120C1C02C}"/>
+    <workbookView xWindow="7680" yWindow="640" windowWidth="28040" windowHeight="17420" activeTab="7" xr2:uid="{2084B393-6D21-FD4B-B70D-EA7120C1C02C}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="16" r:id="rId1"/>
@@ -20,7 +20,7 @@
     <sheet name="gen" sheetId="8" r:id="rId5"/>
     <sheet name="sgen" sheetId="3" r:id="rId6"/>
     <sheet name="asymmetric_sgen" sheetId="6" r:id="rId7"/>
-    <sheet name="fuel" sheetId="17" r:id="rId8"/>
+    <sheet name="fuel" sheetId="19" r:id="rId8"/>
     <sheet name="ext_grid" sheetId="9" r:id="rId9"/>
     <sheet name="storage" sheetId="7" r:id="rId10"/>
     <sheet name="trafo" sheetId="10" r:id="rId11"/>
@@ -834,7 +834,7 @@
   <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="A14" sqref="A14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3227,10 +3227,10 @@
 </file>
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{044941A6-3C9F-0E46-9D3B-A18A4F942C00}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E1D4D7BC-31E7-3D43-A099-A2C290EC3D01}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A40" workbookViewId="0">
       <selection activeCell="K27" sqref="K27"/>
     </sheetView>
   </sheetViews>
@@ -3368,7 +3368,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{446F108F-AC6A-8448-99B0-5E515C432FDC}">
   <dimension ref="A1:G2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="O22" sqref="O22"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>

</xml_diff>

<commit_message>
adjusted scenarios and time series
</commit_message>
<xml_diff>
--- a/example/kerber_landnetz_fl2/scenarios/pv.xlsx
+++ b/example/kerber_landnetz_fl2/scenarios/pv.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/chujiahe/Desktop/propens-pandapower/example/kerber_landnetz_fl2/scenarios/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9783A48A-0E02-4944-B459-9831766DE852}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{59050C02-9178-E144-976B-19F522C0A4AA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2200" yWindow="640" windowWidth="28040" windowHeight="17420" activeTab="5" xr2:uid="{2084B393-6D21-FD4B-B70D-EA7120C1C02C}"/>
+    <workbookView xWindow="2200" yWindow="640" windowWidth="28040" windowHeight="17420" xr2:uid="{2084B393-6D21-FD4B-B70D-EA7120C1C02C}"/>
   </bookViews>
   <sheets>
     <sheet name="general" sheetId="16" r:id="rId1"/>
@@ -53,7 +53,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="320" uniqueCount="141">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="319" uniqueCount="140">
   <si>
     <t>wye</t>
   </si>
@@ -419,9 +419,6 @@
   </si>
   <si>
     <t>household8</t>
-  </si>
-  <si>
-    <t>./example/kerber_landnetz_fl2/timeseries.xlsx</t>
   </si>
   <si>
     <t>solar</t>
@@ -874,8 +871,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{800EF47C-ADD7-984D-8831-B2BC1EF8921F}">
   <dimension ref="A1:D2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G13" sqref="G13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -892,18 +889,15 @@
         <v>112</v>
       </c>
       <c r="C1" s="1" t="s">
+        <v>137</v>
+      </c>
+      <c r="D1" t="s">
         <v>138</v>
-      </c>
-      <c r="D1" t="s">
-        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="b">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>122</v>
+        <v>0</v>
       </c>
       <c r="C2" s="1" t="b">
         <v>0</v>
@@ -2462,16 +2456,16 @@
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
+        <v>127</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>128</v>
       </c>
-      <c r="C1" s="2" t="s">
+      <c r="D1" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="E1" s="2" t="s">
         <v>130</v>
-      </c>
-      <c r="E1" s="2" t="s">
-        <v>131</v>
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.2">
@@ -2497,28 +2491,28 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B1" s="2" t="s">
+        <v>128</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>129</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>130</v>
-      </c>
       <c r="D1" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>132</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="F1" s="2" t="s">
+      <c r="G1" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>136</v>
-      </c>
-      <c r="I1" s="2" t="s">
-        <v>137</v>
       </c>
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
@@ -2576,7 +2570,7 @@
         <v>1</v>
       </c>
       <c r="L1" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:12" ht="16" x14ac:dyDescent="0.2">
@@ -3054,7 +3048,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DC9B8466-B32E-3A45-A8E8-7E7227ADE1CD}">
   <dimension ref="A1:K9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P13" sqref="P13"/>
     </sheetView>
   </sheetViews>
@@ -3092,7 +3086,7 @@
         <v>20</v>
       </c>
       <c r="K1" s="1" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.2">
@@ -3430,13 +3424,13 @@
   <sheetData>
     <row r="1" spans="1:4" s="3" customFormat="1" x14ac:dyDescent="0.2">
       <c r="B1" s="3" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.2">
@@ -3444,13 +3438,13 @@
         <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C2">
         <v>0</v>
       </c>
       <c r="D2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
@@ -3458,13 +3452,13 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C3">
         <v>1</v>
       </c>
       <c r="D3" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
@@ -3472,13 +3466,13 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C4">
         <v>2</v>
       </c>
       <c r="D4" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
@@ -3486,13 +3480,13 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C5">
         <v>3</v>
       </c>
       <c r="D5" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
@@ -3500,13 +3494,13 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C6">
         <v>4</v>
       </c>
       <c r="D6" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.2">
@@ -3514,13 +3508,13 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C7">
         <v>5</v>
       </c>
       <c r="D7" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.2">
@@ -3528,13 +3522,13 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C8">
         <v>6</v>
       </c>
       <c r="D8" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.2">
@@ -3542,13 +3536,13 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="C9">
         <v>7</v>
       </c>
       <c r="D9" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
     </row>
   </sheetData>

</xml_diff>